<commit_message>
Added First Name and Last Name Attribute again in Member and Personal Instructor
</commit_message>
<xml_diff>
--- a/Gym Management System_ER_Table.xlsx
+++ b/Gym Management System_ER_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashr\Desktop\Gym_Management_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE504984-4AEF-49B6-B62F-E13BB241F18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F3FE6A-63B0-4623-AC2F-1DBFC41B6AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="730" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="730" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="11" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="251">
   <si>
     <t>Mem_ID</t>
   </si>
@@ -1635,8 +1635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07ECC70A-237C-4B82-BD44-1242A71A26A6}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2286,40 +2286,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:F12"/>
+      <selection activeCell="B1" sqref="B1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>242</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2338,204 +2345,270 @@
       <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>243</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="2">
+      <c r="F3" s="2">
         <v>43899</v>
       </c>
-      <c r="E3" s="2">
+      <c r="G3" s="2">
         <v>44236</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>244</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2">
+      <c r="F4" s="2">
         <v>43869</v>
       </c>
-      <c r="E4" s="2">
+      <c r="G4" s="2">
         <v>44204</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>224</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="2">
+      <c r="F5" s="2">
         <v>43891</v>
       </c>
-      <c r="E5" s="2">
+      <c r="G5" s="2">
         <v>44228</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>225</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="2">
+      <c r="F6" s="2">
         <v>43899</v>
       </c>
-      <c r="E6" s="2">
+      <c r="G6" s="2">
         <v>44236</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>226</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="2">
+      <c r="F7" s="2">
         <v>44125</v>
       </c>
-      <c r="E7" s="2">
+      <c r="G7" s="2">
         <v>44248</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>232</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="2">
+      <c r="F8" s="2">
         <v>44197</v>
       </c>
-      <c r="E8" s="2">
+      <c r="G8" s="2">
         <v>44228</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>233</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="2">
+      <c r="F9" s="2">
         <v>44090</v>
       </c>
-      <c r="E9" s="2">
+      <c r="G9" s="2">
         <v>44271</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>234</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="2">
+      <c r="F10" s="2">
         <v>44116</v>
       </c>
-      <c r="E10" s="2">
+      <c r="G10" s="2">
         <v>44298</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>235</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="2">
+      <c r="F11" s="2">
         <v>44175</v>
       </c>
-      <c r="E11" s="2">
+      <c r="G11" s="2">
         <v>44206</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>236</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="2">
+      <c r="F12" s="2">
         <v>44179</v>
       </c>
-      <c r="E12" s="2">
+      <c r="G12" s="2">
         <v>44210</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2994,7 +3067,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4102,19 +4175,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>242</v>
       </c>
@@ -4122,10 +4195,16 @@
         <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -4133,116 +4212,182 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>227</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" s="1">
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>228</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E4" s="1">
         <v>4000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>229</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" s="1">
         <v>3000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>230</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="1">
         <v>9000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>231</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E7" s="1">
         <v>4000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>237</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="1">
         <v>5000</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>238</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E9" s="1">
         <v>8000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>239</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E10" s="1">
         <v>7000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>240</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E11" s="1">
         <v>8000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>241</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" s="1">
         <v>5000</v>
       </c>
     </row>
@@ -4255,7 +4400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{741FA951-7562-4920-ABC9-7B63795635E7}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -4386,7 +4531,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>237</v>
       </c>
@@ -4397,7 +4542,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>238</v>
       </c>
@@ -4408,7 +4553,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>238</v>
       </c>
@@ -4419,7 +4564,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>239</v>
       </c>
@@ -4430,7 +4575,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>239</v>
       </c>
@@ -4441,7 +4586,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>240</v>
       </c>
@@ -4452,7 +4597,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>241</v>
       </c>
@@ -4463,7 +4608,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>241</v>
       </c>
@@ -4474,7 +4619,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>241</v>
       </c>
@@ -4485,7 +4630,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>241</v>
       </c>
@@ -4496,7 +4641,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>241</v>
       </c>
@@ -4507,7 +4652,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>241</v>
       </c>

</xml_diff>

<commit_message>
Removed User_ID from Personal_Instructor
</commit_message>
<xml_diff>
--- a/Gym Management System_ER_Table.xlsx
+++ b/Gym Management System_ER_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashr\Desktop\Gym_Management_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F3FE6A-63B0-4623-AC2F-1DBFC41B6AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80F838F-C125-4B39-B58A-F26F434E25CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="730" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="1464" windowWidth="17280" windowHeight="8832" tabRatio="730" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="11" r:id="rId1"/>
@@ -21,14 +21,14 @@
     <sheet name="Monthly_Analysis" sheetId="5" r:id="rId6"/>
     <sheet name="Appoints" sheetId="6" r:id="rId7"/>
     <sheet name="Personal_Instructor" sheetId="7" r:id="rId8"/>
-    <sheet name="Email_IDs" sheetId="10" r:id="rId9"/>
+    <sheet name="Email_ID" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="251">
   <si>
     <t>Mem_ID</t>
   </si>
@@ -2289,7 +2289,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4177,8 +4177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4398,10 +4398,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{741FA951-7562-4920-ABC9-7B63795635E7}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4410,256 +4410,187 @@
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>242</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>227</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="B4" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>228</v>
+        <v>122</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>229</v>
-      </c>
       <c r="B7" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>229</v>
-      </c>
       <c r="B8" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>230</v>
+        <v>123</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="B10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C10" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>231</v>
+        <v>124</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C11" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>237</v>
+        <v>125</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="B13" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>238</v>
+        <v>126</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C14" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>239</v>
+        <v>127</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>239</v>
-      </c>
       <c r="B16" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>240</v>
+        <v>128</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="B18" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>241</v>
+        <v>129</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>241</v>
+        <v>130</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="B21" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="B22" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="B23" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C23" s="1" t="s">
         <v>223</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed column placement of member table of member ID and added all the relax commands
</commit_message>
<xml_diff>
--- a/Gym Management System_ER_Table.xlsx
+++ b/Gym Management System_ER_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashr\Desktop\Gym_Management_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80F838F-C125-4B39-B58A-F26F434E25CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC00A0D7-BD0C-4520-A3D6-A86F0E5B219E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="1464" windowWidth="17280" windowHeight="8832" tabRatio="730" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="730" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="11" r:id="rId1"/>
@@ -1636,7 +1636,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:C22"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2288,8 +2288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2305,13 +2305,13 @@
         <v>242</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>87</v>
@@ -2357,13 +2357,13 @@
         <v>243</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>30</v>
@@ -2383,13 +2383,13 @@
         <v>244</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>30</v>
@@ -2409,13 +2409,13 @@
         <v>224</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>30</v>
@@ -2435,13 +2435,13 @@
         <v>225</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>30</v>
@@ -2461,13 +2461,13 @@
         <v>226</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>44</v>
@@ -2487,13 +2487,13 @@
         <v>232</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>47</v>
@@ -2513,13 +2513,13 @@
         <v>233</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>52</v>
@@ -2539,13 +2539,13 @@
         <v>234</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>52</v>
@@ -2565,13 +2565,13 @@
         <v>235</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>47</v>
@@ -2591,13 +2591,13 @@
         <v>236</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>47</v>
@@ -4400,7 +4400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{741FA951-7562-4920-ABC9-7B63795635E7}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed First_Name, Last_Name from Instructor and Member tables
</commit_message>
<xml_diff>
--- a/Gym Management System_ER_Table.xlsx
+++ b/Gym Management System_ER_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashr\Desktop\Gym_Management_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC00A0D7-BD0C-4520-A3D6-A86F0E5B219E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02C5853-C6F9-453A-8A36-2C9E166C9677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="730" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3324" yWindow="1236" windowWidth="17280" windowHeight="8832" tabRatio="730" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="11" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="251">
   <si>
     <t>Mem_ID</t>
   </si>
@@ -1635,8 +1635,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07ECC70A-237C-4B82-BD44-1242A71A26A6}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2286,10 +2287,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2300,7 +2301,7 @@
     <col min="13" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>242</v>
       </c>
@@ -2308,25 +2309,19 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2345,14 +2340,8 @@
       <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>243</v>
       </c>
@@ -2360,25 +2349,19 @@
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="2">
+      <c r="D3" s="2">
         <v>43899</v>
       </c>
-      <c r="G3" s="2">
+      <c r="E3" s="2">
         <v>44236</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>244</v>
       </c>
@@ -2386,25 +2369,19 @@
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="2">
+      <c r="D4" s="2">
         <v>43869</v>
       </c>
-      <c r="G4" s="2">
+      <c r="E4" s="2">
         <v>44204</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>224</v>
       </c>
@@ -2412,25 +2389,19 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="2">
+      <c r="D5" s="2">
         <v>43891</v>
       </c>
-      <c r="G5" s="2">
+      <c r="E5" s="2">
         <v>44228</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>225</v>
       </c>
@@ -2438,25 +2409,19 @@
         <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="2">
+      <c r="D6" s="2">
         <v>43899</v>
       </c>
-      <c r="G6" s="2">
+      <c r="E6" s="2">
         <v>44236</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>226</v>
       </c>
@@ -2464,25 +2429,19 @@
         <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="2">
+      <c r="D7" s="2">
         <v>44125</v>
       </c>
-      <c r="G7" s="2">
+      <c r="E7" s="2">
         <v>44248</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>232</v>
       </c>
@@ -2490,25 +2449,19 @@
         <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="2">
+      <c r="D8" s="2">
         <v>44197</v>
       </c>
-      <c r="G8" s="2">
+      <c r="E8" s="2">
         <v>44228</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>233</v>
       </c>
@@ -2516,25 +2469,19 @@
         <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="2">
+      <c r="D9" s="2">
         <v>44090</v>
       </c>
-      <c r="G9" s="2">
+      <c r="E9" s="2">
         <v>44271</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>234</v>
       </c>
@@ -2542,25 +2489,19 @@
         <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="2">
+      <c r="D10" s="2">
         <v>44116</v>
       </c>
-      <c r="G10" s="2">
+      <c r="E10" s="2">
         <v>44298</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>235</v>
       </c>
@@ -2568,25 +2509,19 @@
         <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="2">
+      <c r="D11" s="2">
         <v>44175</v>
       </c>
-      <c r="G11" s="2">
+      <c r="E11" s="2">
         <v>44206</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>236</v>
       </c>
@@ -2594,21 +2529,15 @@
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="2">
+      <c r="D12" s="2">
         <v>44179</v>
       </c>
-      <c r="G12" s="2">
+      <c r="E12" s="2">
         <v>44210</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>166</v>
       </c>
     </row>
@@ -4175,10 +4104,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4187,7 +4116,7 @@
     <col min="16" max="16" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>242</v>
       </c>
@@ -4195,16 +4124,10 @@
         <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -4212,182 +4135,116 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>227</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="C3" s="1">
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>228</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="C4" s="1">
         <v>4000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>229</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="C5" s="1">
         <v>3000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>230</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="C6" s="1">
         <v>9000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>231</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="C7" s="1">
         <v>4000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>237</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="C8" s="1">
         <v>5000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>238</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="C9" s="1">
         <v>8000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>239</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="C10" s="1">
         <v>7000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>240</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="C11" s="1">
         <v>8000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>241</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="C12" s="1">
         <v>5000</v>
       </c>
     </row>

</xml_diff>